<commit_message>
Atualizado por script em 03-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/paraguay_primera-division_2023.xlsx
+++ b/2023/paraguay_primera-division_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V105"/>
+  <dimension ref="A1:V107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10117,6 +10117,190 @@
         </is>
       </c>
     </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>paraguay</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>primera-division</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E106" s="2" t="n">
+        <v>45232.91666666666</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Resistencia</t>
+        </is>
+      </c>
+      <c r="G106" t="n">
+        <v>1</v>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Tacuary</t>
+        </is>
+      </c>
+      <c r="I106" t="n">
+        <v>3</v>
+      </c>
+      <c r="J106" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>31/10/2023 00:42</t>
+        </is>
+      </c>
+      <c r="L106" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>02/11/2023 21:58</t>
+        </is>
+      </c>
+      <c r="N106" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>31/10/2023 00:42</t>
+        </is>
+      </c>
+      <c r="P106" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>02/11/2023 21:57</t>
+        </is>
+      </c>
+      <c r="R106" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="S106" t="inlineStr">
+        <is>
+          <t>31/10/2023 00:42</t>
+        </is>
+      </c>
+      <c r="T106" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="U106" t="inlineStr">
+        <is>
+          <t>02/11/2023 21:58</t>
+        </is>
+      </c>
+      <c r="V106" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/paraguay/primera-division/resistencia-tacuary/EBMT9J5K/</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>paraguay</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>primera-division</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E107" s="2" t="n">
+        <v>45233.02083333334</v>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Sportivo Trinidense</t>
+        </is>
+      </c>
+      <c r="G107" t="n">
+        <v>1</v>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Libertad Asuncion</t>
+        </is>
+      </c>
+      <c r="I107" t="n">
+        <v>1</v>
+      </c>
+      <c r="J107" t="n">
+        <v>4.31</v>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>31/10/2023 00:42</t>
+        </is>
+      </c>
+      <c r="L107" t="n">
+        <v>4.64</v>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>03/11/2023 00:24</t>
+        </is>
+      </c>
+      <c r="N107" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>31/10/2023 00:42</t>
+        </is>
+      </c>
+      <c r="P107" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>03/11/2023 00:27</t>
+        </is>
+      </c>
+      <c r="R107" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>31/10/2023 00:42</t>
+        </is>
+      </c>
+      <c r="T107" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="U107" t="inlineStr">
+        <is>
+          <t>03/11/2023 00:21</t>
+        </is>
+      </c>
+      <c r="V107" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/paraguay/primera-division/sportivo-trinidense-libertad-asuncion/roRX8wLQ/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>